<commit_message>
Nurtimax v1 and cvb2022 complete
</commit_message>
<xml_diff>
--- a/scrape-products/Matryca BM3.xlsx
+++ b/scrape-products/Matryca BM3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/Documents/anet/scrape-products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/GitHub/Anet/scrape-products/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE0BFED-9714-EE4D-8863-4107ECAA968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E910DDD-61E2-CD41-A189-CF696CFD7863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20680" yWindow="760" windowWidth="13880" windowHeight="21580" xr2:uid="{DC45400B-429F-2B4B-BE09-71F60257F5F5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{DC45400B-429F-2B4B-BE09-71F60257F5F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,9 +326,6 @@
     <t>%dOMpig</t>
   </si>
   <si>
-    <t>%dNSPpig</t>
-  </si>
-  <si>
     <t>%dPpig</t>
   </si>
   <si>
@@ -929,9 +926,6 @@
     <t>C139</t>
   </si>
   <si>
-    <t>C135</t>
-  </si>
-  <si>
     <t>C027</t>
   </si>
   <si>
@@ -1154,60 +1148,6 @@
     <t>C190</t>
   </si>
   <si>
-    <t>C080</t>
-  </si>
-  <si>
-    <t>C081</t>
-  </si>
-  <si>
-    <t>C082</t>
-  </si>
-  <si>
-    <t>C083</t>
-  </si>
-  <si>
-    <t>C084</t>
-  </si>
-  <si>
-    <t>C085</t>
-  </si>
-  <si>
-    <t>C087</t>
-  </si>
-  <si>
-    <t>C117</t>
-  </si>
-  <si>
-    <t>C118</t>
-  </si>
-  <si>
-    <t>C119</t>
-  </si>
-  <si>
-    <t>C120</t>
-  </si>
-  <si>
-    <t>C086</t>
-  </si>
-  <si>
-    <t>C121</t>
-  </si>
-  <si>
-    <t>C122</t>
-  </si>
-  <si>
-    <t>C123</t>
-  </si>
-  <si>
-    <t>C124</t>
-  </si>
-  <si>
-    <t>C125</t>
-  </si>
-  <si>
-    <t>C126</t>
-  </si>
-  <si>
     <t>C105</t>
   </si>
   <si>
@@ -1266,16 +1206,82 @@
   </si>
   <si>
     <t>&gt;=C20</t>
+  </si>
+  <si>
+    <t>BX272</t>
+  </si>
+  <si>
+    <t>BX273</t>
+  </si>
+  <si>
+    <t>BX274</t>
+  </si>
+  <si>
+    <t>BX275</t>
+  </si>
+  <si>
+    <t>BX276</t>
+  </si>
+  <si>
+    <t>BX277</t>
+  </si>
+  <si>
+    <t>BX278</t>
+  </si>
+  <si>
+    <t>BX279</t>
+  </si>
+  <si>
+    <t>BX280</t>
+  </si>
+  <si>
+    <t>BX281</t>
+  </si>
+  <si>
+    <t>BX282</t>
+  </si>
+  <si>
+    <t>BX283</t>
+  </si>
+  <si>
+    <t>BX284</t>
+  </si>
+  <si>
+    <t>BX285</t>
+  </si>
+  <si>
+    <t>BX286</t>
+  </si>
+  <si>
+    <t>BX287</t>
+  </si>
+  <si>
+    <t>BX288</t>
+  </si>
+  <si>
+    <t>BX289</t>
+  </si>
+  <si>
+    <t>DCNSPh</t>
+  </si>
+  <si>
+    <t>BX290</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1639,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218EEFCF-41A1-094E-BEB9-C87275F12950}">
   <dimension ref="A1:GU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
-      <selection activeCell="DF25" sqref="DF25"/>
+    <sheetView tabSelected="1" topLeftCell="EH1" workbookViewId="0">
+      <selection activeCell="CW11" sqref="CW11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1734,7 @@
         <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="AC1" t="s">
         <v>27</v>
@@ -1755,7 +1761,7 @@
         <v>34</v>
       </c>
       <c r="AK1" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="AL1" t="s">
         <v>35</v>
@@ -2253,1220 +2259,1221 @@
         <v>199</v>
       </c>
       <c r="GU1" t="s">
-        <v>200</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:203" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
         <v>201</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>202</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>203</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>204</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>205</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>206</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>207</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>208</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>209</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>210</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>211</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>212</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>213</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>214</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>215</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>216</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>217</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>218</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>219</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>220</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>221</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>222</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>223</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>224</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>225</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>226</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>227</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>228</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>229</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>230</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>231</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>232</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>233</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>234</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>235</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>236</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>237</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>238</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>239</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>240</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>241</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>242</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>243</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>244</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>245</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
         <v>246</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>247</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>248</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
         <v>249</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>250</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>251</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>252</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>253</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>254</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>255</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>256</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" t="s">
         <v>257</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BI2" t="s">
         <v>258</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BJ2" t="s">
         <v>259</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>260</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BL2" t="s">
         <v>261</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>262</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
         <v>263</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BO2" t="s">
         <v>264</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BP2" t="s">
         <v>265</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
         <v>266</v>
       </c>
-      <c r="BQ2" t="s">
+      <c r="BR2" t="s">
         <v>267</v>
       </c>
-      <c r="BR2" t="s">
+      <c r="BS2" t="s">
         <v>268</v>
       </c>
-      <c r="BS2" t="s">
+      <c r="BT2" t="s">
         <v>269</v>
       </c>
-      <c r="BT2" t="s">
+      <c r="BU2" t="s">
         <v>270</v>
       </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
         <v>271</v>
       </c>
-      <c r="BV2" t="s">
+      <c r="BW2" t="s">
         <v>272</v>
       </c>
-      <c r="BW2" t="s">
+      <c r="BX2" t="s">
         <v>273</v>
       </c>
-      <c r="BX2" t="s">
+      <c r="BY2" t="s">
         <v>274</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="BZ2" t="s">
         <v>275</v>
       </c>
-      <c r="BZ2" t="s">
+      <c r="CA2" t="s">
         <v>276</v>
       </c>
-      <c r="CA2" t="s">
+      <c r="CB2" t="s">
         <v>277</v>
       </c>
-      <c r="CB2" t="s">
+      <c r="CC2" t="s">
         <v>278</v>
       </c>
-      <c r="CC2" t="s">
+      <c r="CD2" t="s">
         <v>279</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CE2" t="s">
         <v>280</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CF2" t="s">
         <v>281</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CG2" t="s">
         <v>282</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CH2" t="s">
         <v>283</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
         <v>284</v>
       </c>
-      <c r="CI2" t="s">
+      <c r="CJ2" t="s">
         <v>285</v>
       </c>
-      <c r="CJ2" t="s">
+      <c r="CK2" t="s">
         <v>286</v>
       </c>
-      <c r="CK2" t="s">
+      <c r="CL2" t="s">
         <v>287</v>
       </c>
-      <c r="CL2" t="s">
+      <c r="CM2" t="s">
         <v>288</v>
       </c>
-      <c r="CM2" t="s">
+      <c r="CN2" t="s">
         <v>289</v>
       </c>
-      <c r="CN2" t="s">
+      <c r="CO2" t="s">
         <v>290</v>
       </c>
-      <c r="CO2" t="s">
+      <c r="CP2" t="s">
         <v>291</v>
       </c>
-      <c r="CP2" t="s">
+      <c r="CQ2" t="s">
         <v>292</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CR2" t="s">
         <v>293</v>
       </c>
-      <c r="CR2" t="s">
+      <c r="CS2" t="s">
         <v>294</v>
       </c>
-      <c r="CS2" t="s">
+      <c r="CT2" t="s">
         <v>295</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CU2" t="s">
         <v>296</v>
       </c>
-      <c r="CU2" t="s">
+      <c r="CV2" t="s">
         <v>297</v>
       </c>
-      <c r="CV2" t="s">
+      <c r="CW2" t="s">
         <v>298</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="CX2" t="s">
         <v>299</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="CY2" t="s">
         <v>300</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="CZ2" t="s">
         <v>301</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="DA2" t="s">
         <v>302</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DB2" t="s">
         <v>303</v>
       </c>
-      <c r="DB2" t="s">
+      <c r="DC2" t="s">
         <v>304</v>
       </c>
-      <c r="DC2" t="s">
+      <c r="DD2" t="s">
         <v>305</v>
       </c>
-      <c r="DD2" t="s">
+      <c r="DE2" t="s">
         <v>306</v>
       </c>
-      <c r="DE2" t="s">
+      <c r="DF2" t="s">
         <v>307</v>
       </c>
-      <c r="DF2" t="s">
+      <c r="DG2" t="s">
         <v>308</v>
       </c>
-      <c r="DG2" t="s">
+      <c r="DH2" t="s">
         <v>309</v>
       </c>
-      <c r="DH2" t="s">
+      <c r="DI2" t="s">
         <v>310</v>
       </c>
-      <c r="DI2" t="s">
+      <c r="DJ2" t="s">
         <v>311</v>
       </c>
-      <c r="DJ2" t="s">
+      <c r="DK2" t="s">
         <v>312</v>
       </c>
-      <c r="DK2" t="s">
+      <c r="DL2" t="s">
         <v>313</v>
       </c>
-      <c r="DL2" t="s">
+      <c r="DM2" t="s">
         <v>314</v>
       </c>
-      <c r="DM2" t="s">
+      <c r="DN2" t="s">
         <v>315</v>
       </c>
-      <c r="DN2" t="s">
+      <c r="DO2" t="s">
         <v>316</v>
       </c>
-      <c r="DO2" t="s">
+      <c r="DP2" t="s">
         <v>317</v>
       </c>
-      <c r="DP2" t="s">
+      <c r="DQ2" t="s">
         <v>318</v>
       </c>
-      <c r="DQ2" t="s">
+      <c r="DR2" t="s">
         <v>319</v>
       </c>
-      <c r="DR2" t="s">
+      <c r="DS2" t="s">
         <v>320</v>
       </c>
-      <c r="DS2" t="s">
+      <c r="DT2" t="s">
         <v>321</v>
       </c>
-      <c r="DT2" t="s">
+      <c r="DU2" t="s">
         <v>322</v>
       </c>
-      <c r="DU2" t="s">
+      <c r="DV2" t="s">
         <v>323</v>
       </c>
-      <c r="DV2" t="s">
+      <c r="DW2" t="s">
         <v>324</v>
       </c>
-      <c r="DW2" t="s">
+      <c r="DX2" t="s">
         <v>325</v>
       </c>
-      <c r="DX2" t="s">
+      <c r="DY2" t="s">
         <v>326</v>
       </c>
-      <c r="DY2" t="s">
+      <c r="DZ2" t="s">
         <v>327</v>
       </c>
-      <c r="DZ2" t="s">
+      <c r="EA2" t="s">
         <v>328</v>
       </c>
-      <c r="EA2" t="s">
+      <c r="EB2" t="s">
         <v>329</v>
       </c>
-      <c r="EB2" t="s">
+      <c r="EC2" t="s">
         <v>330</v>
       </c>
-      <c r="EC2" t="s">
+      <c r="ED2" t="s">
         <v>331</v>
       </c>
-      <c r="ED2" t="s">
+      <c r="EE2" t="s">
         <v>332</v>
       </c>
-      <c r="EE2" t="s">
+      <c r="EF2" t="s">
         <v>333</v>
       </c>
-      <c r="EF2" t="s">
+      <c r="EG2" t="s">
         <v>334</v>
       </c>
-      <c r="EG2" t="s">
+      <c r="EH2" t="s">
         <v>335</v>
       </c>
-      <c r="EH2" t="s">
+      <c r="EI2" t="s">
         <v>336</v>
       </c>
-      <c r="EI2" t="s">
+      <c r="EJ2" t="s">
         <v>337</v>
       </c>
-      <c r="EJ2" t="s">
+      <c r="EK2" t="s">
         <v>338</v>
       </c>
-      <c r="EK2" t="s">
+      <c r="EL2" t="s">
         <v>339</v>
       </c>
-      <c r="EL2" t="s">
+      <c r="EM2" t="s">
         <v>340</v>
       </c>
-      <c r="EM2" t="s">
+      <c r="EN2" t="s">
         <v>341</v>
       </c>
-      <c r="EN2" t="s">
+      <c r="EO2" t="s">
         <v>342</v>
       </c>
-      <c r="EO2" t="s">
+      <c r="EP2" t="s">
         <v>343</v>
       </c>
-      <c r="EP2" t="s">
+      <c r="EQ2" t="s">
         <v>344</v>
       </c>
-      <c r="EQ2" t="s">
+      <c r="ER2" t="s">
         <v>345</v>
       </c>
-      <c r="ER2" t="s">
+      <c r="ES2" t="s">
         <v>346</v>
       </c>
-      <c r="ES2" t="s">
+      <c r="ET2" t="s">
         <v>347</v>
       </c>
-      <c r="ET2" t="s">
+      <c r="EU2" t="s">
         <v>348</v>
       </c>
-      <c r="EU2" t="s">
+      <c r="EV2" t="s">
         <v>349</v>
       </c>
-      <c r="EV2" t="s">
+      <c r="EW2" t="s">
         <v>350</v>
       </c>
-      <c r="EW2" t="s">
+      <c r="EX2" t="s">
         <v>351</v>
       </c>
-      <c r="EX2" t="s">
+      <c r="EY2" t="s">
         <v>352</v>
       </c>
-      <c r="EY2" t="s">
+      <c r="EZ2" t="s">
         <v>353</v>
       </c>
-      <c r="EZ2" t="s">
+      <c r="FA2" t="s">
         <v>354</v>
       </c>
-      <c r="FA2" t="s">
+      <c r="FB2" t="s">
         <v>355</v>
       </c>
-      <c r="FB2" t="s">
+      <c r="FC2" t="s">
         <v>356</v>
       </c>
-      <c r="FC2" t="s">
+      <c r="FD2" t="s">
         <v>357</v>
       </c>
-      <c r="FD2" t="s">
+      <c r="FE2" t="s">
         <v>358</v>
       </c>
-      <c r="FE2" t="s">
+      <c r="FF2" t="s">
         <v>359</v>
       </c>
-      <c r="FF2" t="s">
+      <c r="FG2" t="s">
         <v>360</v>
       </c>
-      <c r="FG2" t="s">
+      <c r="FH2" t="s">
         <v>361</v>
       </c>
-      <c r="FH2" t="s">
+      <c r="FI2" t="s">
         <v>362</v>
       </c>
-      <c r="FI2" t="s">
+      <c r="FJ2" t="s">
         <v>363</v>
       </c>
-      <c r="FJ2" t="s">
+      <c r="FK2" t="s">
         <v>364</v>
       </c>
-      <c r="FK2" t="s">
+      <c r="FL2" t="s">
         <v>365</v>
       </c>
-      <c r="FL2" t="s">
+      <c r="FM2" t="s">
         <v>366</v>
       </c>
-      <c r="FM2" t="s">
+      <c r="FN2" t="s">
         <v>367</v>
       </c>
-      <c r="FN2" t="s">
+      <c r="FO2" t="s">
         <v>368</v>
       </c>
-      <c r="FO2" t="s">
+      <c r="FP2" t="s">
         <v>369</v>
       </c>
-      <c r="FP2" t="s">
+      <c r="FQ2" t="s">
+        <v>390</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>391</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>392</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>393</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>394</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>395</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>396</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>397</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>398</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>399</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>400</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>401</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>402</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>403</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>404</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>405</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>406</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>407</v>
+      </c>
+      <c r="GI2" t="s">
         <v>370</v>
       </c>
-      <c r="FQ2" t="s">
+      <c r="GJ2" t="s">
         <v>371</v>
       </c>
-      <c r="FR2" t="s">
+      <c r="GK2" t="s">
         <v>372</v>
       </c>
-      <c r="FS2" t="s">
+      <c r="GL2" t="s">
         <v>373</v>
       </c>
-      <c r="FT2" t="s">
+      <c r="GM2" t="s">
         <v>374</v>
       </c>
-      <c r="FU2" t="s">
+      <c r="GN2" t="s">
         <v>375</v>
       </c>
-      <c r="FV2" t="s">
+      <c r="GO2" t="s">
         <v>376</v>
       </c>
-      <c r="FW2" t="s">
+      <c r="GP2" t="s">
         <v>377</v>
       </c>
-      <c r="FX2" t="s">
+      <c r="GQ2" t="s">
         <v>378</v>
       </c>
-      <c r="FY2" t="s">
+      <c r="GR2" t="s">
         <v>379</v>
       </c>
-      <c r="FZ2" t="s">
+      <c r="GS2" t="s">
         <v>380</v>
       </c>
-      <c r="GA2" t="s">
+      <c r="GT2" t="s">
         <v>381</v>
       </c>
-      <c r="GB2" t="s">
-        <v>382</v>
-      </c>
-      <c r="GC2" t="s">
-        <v>383</v>
-      </c>
-      <c r="GD2" t="s">
-        <v>384</v>
-      </c>
-      <c r="GE2" t="s">
-        <v>385</v>
-      </c>
-      <c r="GF2" t="s">
-        <v>386</v>
-      </c>
-      <c r="GG2" t="s">
-        <v>387</v>
-      </c>
-      <c r="GH2" t="s">
-        <v>388</v>
-      </c>
-      <c r="GI2" t="s">
-        <v>389</v>
-      </c>
-      <c r="GJ2" t="s">
-        <v>390</v>
-      </c>
-      <c r="GK2" t="s">
-        <v>391</v>
-      </c>
-      <c r="GL2" t="s">
-        <v>392</v>
-      </c>
-      <c r="GM2" t="s">
-        <v>393</v>
-      </c>
-      <c r="GN2" t="s">
-        <v>394</v>
-      </c>
-      <c r="GO2" t="s">
-        <v>395</v>
-      </c>
-      <c r="GP2" t="s">
-        <v>396</v>
-      </c>
-      <c r="GQ2" t="s">
-        <v>397</v>
-      </c>
-      <c r="GR2" t="s">
-        <v>398</v>
-      </c>
-      <c r="GS2" t="s">
-        <v>399</v>
-      </c>
-      <c r="GT2" t="s">
-        <v>400</v>
-      </c>
       <c r="GU2" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:203" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="D3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="E3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="F3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="G3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="H3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="I3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="J3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="K3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="L3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="M3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="N3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="O3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="P3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="Q3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="R3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="S3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="T3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="U3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="V3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="W3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="X3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="Y3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="Z3" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="AA3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AB3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AC3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AD3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AE3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AF3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AG3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AH3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AI3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AJ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AK3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AL3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="AM3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AN3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AO3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AP3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AQ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AR3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AS3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AT3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AV3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AW3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AX3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AY3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="AZ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="BA3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BB3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BC3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BD3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BE3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BF3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BG3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BH3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BI3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BJ3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BK3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BL3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BM3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BN3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BO3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BP3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BQ3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BR3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BS3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BT3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="BU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="BV3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="BW3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="BX3" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="BY3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="BZ3" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="CA3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CB3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CC3" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="CD3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CE3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CF3" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="CG3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CH3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CI3" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="CJ3" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="CK3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CL3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CM3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CN3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CO3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CP3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CQ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CR3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CS3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CT3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CV3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="CW3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="CX3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CY3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="CZ3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DA3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DB3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DC3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DD3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DE3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DF3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DG3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DH3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DI3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="DJ3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="DK3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DL3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DM3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DN3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DO3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DP3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DQ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DR3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DS3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DT3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DV3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DW3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DX3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DY3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="DZ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EA3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EB3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EC3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="ED3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EE3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EF3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EG3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="EH3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="EI3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EJ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EK3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="EL3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EM3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EN3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EO3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EP3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EQ3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="ER3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="ES3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="ET3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="EU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EV3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="EW3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="EX3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EY3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="EZ3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="FA3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="FB3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="FC3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="FD3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="FE3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="FF3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FG3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FH3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FI3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FJ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FK3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FL3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FM3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FN3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FO3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FP3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="FQ3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="FR3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FS3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FT3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FV3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FW3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FX3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FY3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="FZ3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GA3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GB3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GC3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GD3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GE3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GF3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GG3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GH3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GI3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="GJ3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="GK3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GL3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GM3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GN3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="GO3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="GP3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="GQ3" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="GR3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="GS3" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="GT3" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="GU3" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>